<commit_message>
primera corrida de pep8
</commit_message>
<xml_diff>
--- a/tests/results/catalog/example/catalog.xlsx
+++ b/tests/results/catalog/example/catalog.xlsx
@@ -2,6 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="145">
   <si>
     <t>catalog_identifier</t>
   </si>
@@ -86,6 +87,9 @@
     <t>spa</t>
   </si>
   <si>
+    <t>http://datos.gob.ar/superThemeTaxonomy.json</t>
+  </si>
+  <si>
     <t>Open Data Commons Open Database License 1.0</t>
   </si>
   <si>
@@ -254,6 +258,9 @@
     <t>distribution_rights</t>
   </si>
   <si>
+    <t>distribution_type</t>
+  </si>
+  <si>
     <t>Convocatorias abiertas durante el año 2015</t>
   </si>
   <si>
@@ -275,6 +282,9 @@
     <t>text/csv</t>
   </si>
   <si>
+    <t>file</t>
+  </si>
+  <si>
     <t>d_7d4d816f-3a40-476e-ab71-d48a3f0eb3c8</t>
   </si>
   <si>
@@ -288,6 +298,9 @@
   </si>
   <si>
     <t>application/pdf</t>
+  </si>
+  <si>
+    <t>documentation</t>
   </si>
   <si>
     <t>field_title</t>
@@ -853,20 +866,23 @@
       <c r="H2" t="s">
         <v>21</v>
       </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -890,99 +906,99 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="T1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
         <v>19</v>
@@ -994,54 +1010,54 @@
         <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
         <v>19</v>
@@ -1053,19 +1069,19 @@
         <v>21</v>
       </c>
       <c r="O3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1079,7 +1095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1087,86 +1103,89 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" t="n">
         <v>5120</v>
@@ -1178,42 +1197,45 @@
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s">
         <v>85</v>
       </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" t="s">
-        <v>83</v>
-      </c>
       <c r="J3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" t="n">
         <v>5120</v>
@@ -1225,7 +1247,10 @@
         <v>20</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1249,284 +1274,284 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" t="s">
         <v>107</v>
       </c>
-      <c r="F7" t="s">
-        <v>103</v>
-      </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G9" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G10" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1550,79 +1575,79 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>